<commit_message>
09/24/24 commit - updated overall PDF
</commit_message>
<xml_diff>
--- a/public/results/Bottoms Up 2024 League Stats - Week 21.xlsx
+++ b/public/results/Bottoms Up 2024 League Stats - Week 21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\CODE\golf-league-site\public\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7E0643-3513-4A94-B9AB-459703A44386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECE393D-A9A6-47A7-911B-D8686E5E4F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="615" windowWidth="20400" windowHeight="13695" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1995" yWindow="720" windowWidth="20400" windowHeight="13695" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OVERALL" sheetId="30" r:id="rId1"/>
@@ -1520,7 +1520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="257">
+  <cellXfs count="254">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2024,6 +2024,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2061,6 +2097,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2072,63 +2117,6 @@
     </xf>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2175,6 +2163,54 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2185,51 +2221,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2711,34 +2702,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="187"/>
-      <c r="B1" s="188"/>
-      <c r="C1" s="189"/>
-      <c r="D1" s="189"/>
-      <c r="E1" s="189"/>
-      <c r="F1" s="190"/>
-      <c r="H1" s="191" t="s">
+      <c r="A1" s="199"/>
+      <c r="B1" s="200"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="202"/>
+      <c r="H1" s="203" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="192"/>
-      <c r="J1" s="193"/>
+      <c r="I1" s="204"/>
+      <c r="J1" s="205"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="163"/>
       <c r="B2" s="164"/>
-      <c r="C2" s="194" t="s">
+      <c r="C2" s="206" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="195"/>
-      <c r="E2" s="194" t="s">
+      <c r="D2" s="207"/>
+      <c r="E2" s="206" t="s">
         <v>125</v>
       </c>
-      <c r="F2" s="195"/>
-      <c r="H2" s="194" t="s">
+      <c r="F2" s="207"/>
+      <c r="H2" s="206" t="s">
         <v>126</v>
       </c>
-      <c r="I2" s="196"/>
-      <c r="J2" s="195"/>
+      <c r="I2" s="208"/>
+      <c r="J2" s="207"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="165"/>
@@ -2775,7 +2766,7 @@
       <c r="C4" s="173">
         <v>0</v>
       </c>
-      <c r="D4" s="249">
+      <c r="D4" s="191">
         <v>0</v>
       </c>
       <c r="E4" s="186">
@@ -2785,15 +2776,15 @@
         <v>6</v>
       </c>
       <c r="H4" s="175">
-        <f>C4+E4</f>
+        <f t="shared" ref="H4:H21" si="0">C4+E4</f>
         <v>119</v>
       </c>
-      <c r="I4" s="252">
-        <f>D4+F4</f>
+      <c r="I4" s="194">
+        <f t="shared" ref="I4:I21" si="1">D4+F4</f>
         <v>6</v>
       </c>
       <c r="J4" s="176">
-        <f>H4/I4</f>
+        <f t="shared" ref="J4:J21" si="2">H4/I4</f>
         <v>19.833333333333332</v>
       </c>
     </row>
@@ -2813,19 +2804,19 @@
       <c r="E5" s="179">
         <v>105</v>
       </c>
-      <c r="F5" s="250">
+      <c r="F5" s="192">
         <v>5</v>
       </c>
       <c r="H5" s="180">
-        <f>C5+E5</f>
+        <f t="shared" si="0"/>
         <v>271</v>
       </c>
       <c r="I5" s="3">
-        <f>D5+F5</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="J5" s="181">
-        <f>H5/I5</f>
+        <f t="shared" si="2"/>
         <v>19.357142857142858</v>
       </c>
     </row>
@@ -2845,19 +2836,19 @@
       <c r="E6" s="177">
         <v>99</v>
       </c>
-      <c r="F6" s="250">
+      <c r="F6" s="192">
         <v>5</v>
       </c>
       <c r="H6" s="180">
-        <f>C6+E6</f>
+        <f t="shared" si="0"/>
         <v>305</v>
       </c>
       <c r="I6" s="3">
-        <f>D6+F6</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="J6" s="181">
-        <f>H6/I6</f>
+        <f t="shared" si="2"/>
         <v>19.0625</v>
       </c>
     </row>
@@ -2881,15 +2872,15 @@
         <v>7</v>
       </c>
       <c r="H7" s="180">
-        <f>C7+E7</f>
+        <f t="shared" si="0"/>
         <v>265</v>
       </c>
       <c r="I7" s="3">
-        <f>D7+F7</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="J7" s="181">
-        <f>H7/I7</f>
+        <f t="shared" si="2"/>
         <v>18.928571428571427</v>
       </c>
     </row>
@@ -2909,19 +2900,19 @@
       <c r="E8" s="179">
         <v>0</v>
       </c>
-      <c r="F8" s="250">
+      <c r="F8" s="192">
         <v>0</v>
       </c>
       <c r="H8" s="180">
-        <f>C8+E8</f>
+        <f t="shared" si="0"/>
         <v>169</v>
       </c>
-      <c r="I8" s="253">
-        <f>D8+F8</f>
+      <c r="I8" s="195">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J8" s="181">
-        <f>H8/I8</f>
+        <f t="shared" si="2"/>
         <v>18.777777777777779</v>
       </c>
     </row>
@@ -2945,15 +2936,15 @@
         <v>8</v>
       </c>
       <c r="H9" s="180">
-        <f>C9+E9</f>
+        <f t="shared" si="0"/>
         <v>281</v>
       </c>
       <c r="I9" s="3">
-        <f>D9+F9</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="J9" s="181">
-        <f>H9/I9</f>
+        <f t="shared" si="2"/>
         <v>18.733333333333334</v>
       </c>
     </row>
@@ -2977,15 +2968,15 @@
         <v>6</v>
       </c>
       <c r="H10" s="180">
-        <f>C10+E10</f>
+        <f t="shared" si="0"/>
         <v>222</v>
       </c>
       <c r="I10" s="3">
-        <f>D10+F10</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="J10" s="181">
-        <f>H10/I10</f>
+        <f t="shared" si="2"/>
         <v>18.5</v>
       </c>
     </row>
@@ -3009,15 +3000,15 @@
         <v>6</v>
       </c>
       <c r="H11" s="180">
-        <f>C11+E11</f>
+        <f t="shared" si="0"/>
         <v>240</v>
       </c>
       <c r="I11" s="3">
-        <f>D11+F11</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="J11" s="181">
-        <f>H11/I11</f>
+        <f t="shared" si="2"/>
         <v>18.46153846153846</v>
       </c>
     </row>
@@ -3041,15 +3032,15 @@
         <v>8</v>
       </c>
       <c r="H12" s="180">
-        <f>C12+E12</f>
+        <f t="shared" si="0"/>
         <v>328</v>
       </c>
       <c r="I12" s="3">
-        <f>D12+F12</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="J12" s="181">
-        <f>H12/I12</f>
+        <f t="shared" si="2"/>
         <v>18.222222222222221</v>
       </c>
     </row>
@@ -3063,25 +3054,25 @@
       <c r="C13" s="177">
         <v>88</v>
       </c>
-      <c r="D13" s="250">
+      <c r="D13" s="192">
         <v>5</v>
       </c>
       <c r="E13" s="179">
         <v>74</v>
       </c>
-      <c r="F13" s="250">
+      <c r="F13" s="192">
         <v>4</v>
       </c>
       <c r="H13" s="180">
-        <f>C13+E13</f>
+        <f t="shared" si="0"/>
         <v>162</v>
       </c>
-      <c r="I13" s="253">
-        <f>D13+F13</f>
+      <c r="I13" s="195">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J13" s="181">
-        <f>H13/I13</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
     </row>
@@ -3095,25 +3086,25 @@
       <c r="C14" s="177">
         <v>72</v>
       </c>
-      <c r="D14" s="250">
+      <c r="D14" s="192">
         <v>4</v>
       </c>
       <c r="E14" s="179">
         <v>0</v>
       </c>
-      <c r="F14" s="250">
+      <c r="F14" s="192">
         <v>0</v>
       </c>
       <c r="H14" s="180">
-        <f>C14+E14</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="I14" s="253">
-        <f>D14+F14</f>
+      <c r="I14" s="195">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J14" s="181">
-        <f>H14/I14</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
     </row>
@@ -3133,19 +3124,19 @@
       <c r="E15" s="179">
         <v>66</v>
       </c>
-      <c r="F15" s="250">
+      <c r="F15" s="192">
         <v>4</v>
       </c>
       <c r="H15" s="180">
-        <f>C15+E15</f>
+        <f t="shared" si="0"/>
         <v>212</v>
       </c>
       <c r="I15" s="3">
-        <f>D15+F15</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="J15" s="181">
-        <f>H15/I15</f>
+        <f t="shared" si="2"/>
         <v>17.666666666666668</v>
       </c>
     </row>
@@ -3169,15 +3160,15 @@
         <v>7</v>
       </c>
       <c r="H16" s="180">
-        <f>C16+E16</f>
+        <f t="shared" si="0"/>
         <v>280</v>
       </c>
       <c r="I16" s="3">
-        <f>D16+F16</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="J16" s="181">
-        <f>H16/I16</f>
+        <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
     </row>
@@ -3197,19 +3188,19 @@
       <c r="E17" s="179">
         <v>71</v>
       </c>
-      <c r="F17" s="250">
+      <c r="F17" s="192">
         <v>4</v>
       </c>
       <c r="H17" s="180">
-        <f>C17+E17</f>
+        <f t="shared" si="0"/>
         <v>173</v>
       </c>
-      <c r="I17" s="253">
-        <f>D17+F17</f>
+      <c r="I17" s="195">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="J17" s="181">
-        <f>H17/I17</f>
+        <f t="shared" si="2"/>
         <v>17.3</v>
       </c>
     </row>
@@ -3223,25 +3214,25 @@
       <c r="C18" s="177">
         <v>0</v>
       </c>
-      <c r="D18" s="250">
+      <c r="D18" s="192">
         <v>1</v>
       </c>
       <c r="E18" s="179">
         <v>0</v>
       </c>
-      <c r="F18" s="250">
+      <c r="F18" s="192">
         <v>1</v>
       </c>
       <c r="H18" s="180">
-        <f>C18+E18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I18" s="253">
-        <f>D18+F18</f>
+      <c r="I18" s="195">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J18" s="181">
-        <f>H18/I18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3255,25 +3246,25 @@
       <c r="C19" s="177">
         <v>0</v>
       </c>
-      <c r="D19" s="250">
+      <c r="D19" s="192">
         <v>1</v>
       </c>
       <c r="E19" s="179">
         <v>0</v>
       </c>
-      <c r="F19" s="250">
+      <c r="F19" s="192">
         <v>0</v>
       </c>
       <c r="H19" s="180">
-        <f>C19+E19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I19" s="253">
-        <f>D19+F19</f>
+      <c r="I19" s="195">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J19" s="181">
-        <f>H19/I19</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3287,25 +3278,25 @@
       <c r="C20" s="177">
         <v>0</v>
       </c>
-      <c r="D20" s="250">
+      <c r="D20" s="192">
         <v>0</v>
       </c>
       <c r="E20" s="179">
         <v>0</v>
       </c>
-      <c r="F20" s="250">
+      <c r="F20" s="192">
         <v>1</v>
       </c>
       <c r="H20" s="180">
-        <f>C20+E20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I20" s="253">
-        <f>D20+F20</f>
+      <c r="I20" s="195">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J20" s="181">
-        <f>H20/I20</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3319,35 +3310,35 @@
       <c r="C21" s="182">
         <v>0</v>
       </c>
-      <c r="D21" s="251">
+      <c r="D21" s="193">
         <v>1</v>
       </c>
       <c r="E21" s="183">
         <v>0</v>
       </c>
-      <c r="F21" s="251">
+      <c r="F21" s="193">
         <v>0</v>
       </c>
       <c r="H21" s="184">
-        <f>C21+E21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I21" s="254">
-        <f>D21+F21</f>
+      <c r="I21" s="196">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J21" s="170">
-        <f>H21/I21</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="256"/>
-      <c r="D23" s="255" t="s">
+      <c r="C23" s="197"/>
+      <c r="D23" s="198" t="s">
         <v>131</v>
       </c>
-      <c r="E23" s="255"/>
-      <c r="F23" s="255"/>
+      <c r="E23" s="198"/>
+      <c r="F23" s="198"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J21">
@@ -3396,23 +3387,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -3426,23 +3417,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -5070,23 +5061,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -5100,23 +5091,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -6125,23 +6116,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -6155,23 +6146,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -7177,23 +7168,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -7207,23 +7198,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -8614,23 +8605,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -8644,23 +8635,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -9666,23 +9657,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -9696,23 +9687,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -10615,23 +10606,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -10645,23 +10636,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -11981,23 +11972,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -12011,23 +12002,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -13338,24 +13329,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="241" t="s">
+      <c r="A1" s="253" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="241"/>
-      <c r="C1" s="241"/>
-      <c r="D1" s="241"/>
+      <c r="B1" s="253"/>
+      <c r="C1" s="253"/>
+      <c r="D1" s="253"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="241"/>
-      <c r="B2" s="241"/>
-      <c r="C2" s="241"/>
-      <c r="D2" s="241"/>
+      <c r="A2" s="253"/>
+      <c r="B2" s="253"/>
+      <c r="C2" s="253"/>
+      <c r="D2" s="253"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="241"/>
-      <c r="B3" s="241"/>
-      <c r="C3" s="241"/>
-      <c r="D3" s="241"/>
+      <c r="A3" s="253"/>
+      <c r="B3" s="253"/>
+      <c r="C3" s="253"/>
+      <c r="D3" s="253"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -13392,23 +13383,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -13422,23 +13413,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -14764,23 +14755,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -14794,23 +14785,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -15653,24 +15644,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="241" t="s">
+      <c r="A1" s="253" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="241"/>
-      <c r="C1" s="241"/>
-      <c r="D1" s="241"/>
+      <c r="B1" s="253"/>
+      <c r="C1" s="253"/>
+      <c r="D1" s="253"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="241"/>
-      <c r="B2" s="241"/>
-      <c r="C2" s="241"/>
-      <c r="D2" s="241"/>
+      <c r="A2" s="253"/>
+      <c r="B2" s="253"/>
+      <c r="C2" s="253"/>
+      <c r="D2" s="253"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="241"/>
-      <c r="B3" s="241"/>
-      <c r="C3" s="241"/>
-      <c r="D3" s="241"/>
+      <c r="A3" s="253"/>
+      <c r="B3" s="253"/>
+      <c r="C3" s="253"/>
+      <c r="D3" s="253"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -15707,23 +15698,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -15737,23 +15728,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -17077,23 +17068,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -17107,23 +17098,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -18400,23 +18391,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -18430,23 +18421,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -19723,23 +19714,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -19753,23 +19744,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -21035,23 +21026,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -21065,23 +21056,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -22100,244 +22091,244 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" s="1" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="206" t="s">
+      <c r="A1" s="237" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="207"/>
-      <c r="C1" s="212"/>
-      <c r="D1" s="215" t="s">
+      <c r="B1" s="238"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="246" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="200" t="s">
+      <c r="E1" s="215" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="201"/>
-      <c r="G1" s="200" t="s">
+      <c r="F1" s="216"/>
+      <c r="G1" s="215" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="201"/>
-      <c r="I1" s="200" t="s">
+      <c r="H1" s="216"/>
+      <c r="I1" s="215" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="201"/>
-      <c r="K1" s="200" t="s">
+      <c r="J1" s="216"/>
+      <c r="K1" s="215" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="201"/>
-      <c r="M1" s="200" t="s">
+      <c r="L1" s="216"/>
+      <c r="M1" s="215" t="s">
         <v>70</v>
       </c>
-      <c r="N1" s="201"/>
-      <c r="O1" s="200" t="s">
+      <c r="N1" s="216"/>
+      <c r="O1" s="215" t="s">
         <v>84</v>
       </c>
-      <c r="P1" s="201"/>
-      <c r="Q1" s="200" t="s">
+      <c r="P1" s="216"/>
+      <c r="Q1" s="215" t="s">
         <v>89</v>
       </c>
-      <c r="R1" s="201"/>
-      <c r="S1" s="200" t="s">
+      <c r="R1" s="216"/>
+      <c r="S1" s="215" t="s">
         <v>90</v>
       </c>
-      <c r="T1" s="201"/>
-      <c r="U1" s="200" t="s">
+      <c r="T1" s="216"/>
+      <c r="U1" s="215" t="s">
         <v>93</v>
       </c>
-      <c r="V1" s="201"/>
-      <c r="W1" s="200" t="s">
+      <c r="V1" s="216"/>
+      <c r="W1" s="215" t="s">
         <v>95</v>
       </c>
-      <c r="X1" s="201"/>
-      <c r="Y1" s="200" t="s">
+      <c r="X1" s="216"/>
+      <c r="Y1" s="215" t="s">
         <v>96</v>
       </c>
-      <c r="Z1" s="201"/>
-      <c r="AA1" s="200" t="s">
+      <c r="Z1" s="216"/>
+      <c r="AA1" s="215" t="s">
         <v>105</v>
       </c>
-      <c r="AB1" s="201"/>
-      <c r="AC1" s="200" t="s">
+      <c r="AB1" s="216"/>
+      <c r="AC1" s="215" t="s">
         <v>110</v>
       </c>
-      <c r="AD1" s="201"/>
-      <c r="AE1" s="200" t="s">
+      <c r="AD1" s="216"/>
+      <c r="AE1" s="215" t="s">
         <v>112</v>
       </c>
-      <c r="AF1" s="201"/>
-      <c r="AG1" s="200" t="s">
+      <c r="AF1" s="216"/>
+      <c r="AG1" s="215" t="s">
         <v>113</v>
       </c>
-      <c r="AH1" s="201"/>
-      <c r="AI1" s="200" t="s">
+      <c r="AH1" s="216"/>
+      <c r="AI1" s="215" t="s">
         <v>115</v>
       </c>
-      <c r="AJ1" s="201"/>
-      <c r="AK1" s="200" t="s">
+      <c r="AJ1" s="216"/>
+      <c r="AK1" s="215" t="s">
         <v>116</v>
       </c>
-      <c r="AL1" s="201"/>
-      <c r="AM1" s="200" t="s">
+      <c r="AL1" s="216"/>
+      <c r="AM1" s="215" t="s">
         <v>118</v>
       </c>
-      <c r="AN1" s="201"/>
-      <c r="AO1" s="200" t="s">
+      <c r="AN1" s="216"/>
+      <c r="AO1" s="215" t="s">
         <v>119</v>
       </c>
-      <c r="AP1" s="201"/>
-      <c r="AQ1" s="200" t="s">
+      <c r="AP1" s="216"/>
+      <c r="AQ1" s="215" t="s">
         <v>120</v>
       </c>
-      <c r="AR1" s="201"/>
-      <c r="AS1" s="200" t="s">
+      <c r="AR1" s="216"/>
+      <c r="AS1" s="215" t="s">
         <v>129</v>
       </c>
-      <c r="AT1" s="201"/>
-      <c r="AU1" s="217" t="s">
+      <c r="AT1" s="216"/>
+      <c r="AU1" s="234" t="s">
         <v>35</v>
       </c>
-      <c r="AV1" s="226" t="s">
+      <c r="AV1" s="222" t="s">
         <v>111</v>
       </c>
       <c r="AW1" s="112"/>
-      <c r="AX1" s="229" t="s">
+      <c r="AX1" s="225" t="s">
         <v>103</v>
       </c>
-      <c r="AY1" s="230"/>
-      <c r="AZ1" s="230"/>
-      <c r="BA1" s="231"/>
-      <c r="BB1" s="220" t="s">
+      <c r="AY1" s="226"/>
+      <c r="AZ1" s="226"/>
+      <c r="BA1" s="227"/>
+      <c r="BB1" s="212" t="s">
         <v>109</v>
       </c>
-      <c r="BC1" s="223" t="s">
+      <c r="BC1" s="219" t="s">
         <v>104</v>
       </c>
-      <c r="BD1" s="224"/>
-      <c r="BE1" s="224"/>
-      <c r="BF1" s="225"/>
+      <c r="BD1" s="220"/>
+      <c r="BE1" s="220"/>
+      <c r="BF1" s="221"/>
     </row>
     <row r="2" spans="1:58" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="208"/>
-      <c r="B2" s="209"/>
-      <c r="C2" s="213"/>
-      <c r="D2" s="216"/>
-      <c r="E2" s="202">
+      <c r="A2" s="239"/>
+      <c r="B2" s="240"/>
+      <c r="C2" s="244"/>
+      <c r="D2" s="247"/>
+      <c r="E2" s="217">
         <v>45418</v>
       </c>
-      <c r="F2" s="203"/>
-      <c r="G2" s="204">
+      <c r="F2" s="218"/>
+      <c r="G2" s="248">
         <v>45425</v>
       </c>
-      <c r="H2" s="205"/>
-      <c r="I2" s="204">
+      <c r="H2" s="249"/>
+      <c r="I2" s="248">
         <v>45432</v>
       </c>
-      <c r="J2" s="205"/>
-      <c r="K2" s="204">
+      <c r="J2" s="249"/>
+      <c r="K2" s="248">
         <v>45439</v>
       </c>
-      <c r="L2" s="205"/>
-      <c r="M2" s="204">
+      <c r="L2" s="249"/>
+      <c r="M2" s="248">
         <v>45446</v>
       </c>
-      <c r="N2" s="205"/>
-      <c r="O2" s="204">
+      <c r="N2" s="249"/>
+      <c r="O2" s="248">
         <v>45453</v>
       </c>
-      <c r="P2" s="205"/>
-      <c r="Q2" s="204">
+      <c r="P2" s="249"/>
+      <c r="Q2" s="248">
         <v>45460</v>
       </c>
-      <c r="R2" s="205"/>
-      <c r="S2" s="204">
+      <c r="R2" s="249"/>
+      <c r="S2" s="248">
         <v>45467</v>
       </c>
-      <c r="T2" s="205"/>
-      <c r="U2" s="204">
+      <c r="T2" s="249"/>
+      <c r="U2" s="248">
         <v>45474</v>
       </c>
-      <c r="V2" s="205"/>
-      <c r="W2" s="204">
+      <c r="V2" s="249"/>
+      <c r="W2" s="248">
         <v>45481</v>
       </c>
-      <c r="X2" s="205"/>
-      <c r="Y2" s="204">
+      <c r="X2" s="249"/>
+      <c r="Y2" s="248">
         <v>45488</v>
       </c>
-      <c r="Z2" s="205"/>
-      <c r="AA2" s="202">
+      <c r="Z2" s="249"/>
+      <c r="AA2" s="217">
         <v>45495</v>
       </c>
-      <c r="AB2" s="203"/>
-      <c r="AC2" s="202">
+      <c r="AB2" s="218"/>
+      <c r="AC2" s="217">
         <v>45502</v>
       </c>
-      <c r="AD2" s="203"/>
-      <c r="AE2" s="202">
+      <c r="AD2" s="218"/>
+      <c r="AE2" s="217">
         <v>45509</v>
       </c>
-      <c r="AF2" s="203"/>
-      <c r="AG2" s="202">
+      <c r="AF2" s="218"/>
+      <c r="AG2" s="217">
         <v>45516</v>
       </c>
-      <c r="AH2" s="203"/>
-      <c r="AI2" s="202">
+      <c r="AH2" s="218"/>
+      <c r="AI2" s="217">
         <v>45523</v>
       </c>
-      <c r="AJ2" s="203"/>
-      <c r="AK2" s="202">
+      <c r="AJ2" s="218"/>
+      <c r="AK2" s="217">
         <v>45530</v>
       </c>
-      <c r="AL2" s="203"/>
-      <c r="AM2" s="202">
+      <c r="AL2" s="218"/>
+      <c r="AM2" s="217">
         <v>45537</v>
       </c>
-      <c r="AN2" s="203"/>
-      <c r="AO2" s="202">
+      <c r="AN2" s="218"/>
+      <c r="AO2" s="217">
         <v>45544</v>
       </c>
-      <c r="AP2" s="203"/>
-      <c r="AQ2" s="202">
+      <c r="AP2" s="218"/>
+      <c r="AQ2" s="217">
         <v>45551</v>
       </c>
-      <c r="AR2" s="203"/>
-      <c r="AS2" s="202">
+      <c r="AR2" s="218"/>
+      <c r="AS2" s="217">
         <v>45558</v>
       </c>
-      <c r="AT2" s="203"/>
-      <c r="AU2" s="218"/>
-      <c r="AV2" s="227"/>
+      <c r="AT2" s="218"/>
+      <c r="AU2" s="235"/>
+      <c r="AV2" s="223"/>
       <c r="AW2" s="112"/>
-      <c r="AX2" s="232" t="s">
+      <c r="AX2" s="228" t="s">
         <v>88</v>
       </c>
-      <c r="AY2" s="234" t="s">
+      <c r="AY2" s="230" t="s">
         <v>102</v>
       </c>
-      <c r="AZ2" s="234" t="s">
+      <c r="AZ2" s="230" t="s">
         <v>36</v>
       </c>
-      <c r="BA2" s="236" t="s">
+      <c r="BA2" s="232" t="s">
         <v>61</v>
       </c>
-      <c r="BB2" s="221"/>
-      <c r="BC2" s="220" t="s">
+      <c r="BB2" s="213"/>
+      <c r="BC2" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="BD2" s="220" t="s">
+      <c r="BD2" s="212" t="s">
         <v>102</v>
       </c>
-      <c r="BE2" s="220" t="s">
+      <c r="BE2" s="212" t="s">
         <v>36</v>
       </c>
-      <c r="BF2" s="220" t="s">
+      <c r="BF2" s="212" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:58" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="210"/>
-      <c r="B3" s="211"/>
-      <c r="C3" s="214"/>
-      <c r="D3" s="216"/>
+      <c r="A3" s="241"/>
+      <c r="B3" s="242"/>
+      <c r="C3" s="245"/>
+      <c r="D3" s="247"/>
       <c r="E3" s="52" t="s">
         <v>26</v>
       </c>
@@ -22464,18 +22455,18 @@
       <c r="AT3" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="AU3" s="219"/>
-      <c r="AV3" s="228"/>
+      <c r="AU3" s="236"/>
+      <c r="AV3" s="224"/>
       <c r="AW3" s="112"/>
-      <c r="AX3" s="233"/>
-      <c r="AY3" s="235"/>
-      <c r="AZ3" s="235"/>
-      <c r="BA3" s="237"/>
-      <c r="BB3" s="222"/>
-      <c r="BC3" s="221"/>
-      <c r="BD3" s="221"/>
-      <c r="BE3" s="221"/>
-      <c r="BF3" s="221"/>
+      <c r="AX3" s="229"/>
+      <c r="AY3" s="231"/>
+      <c r="AZ3" s="231"/>
+      <c r="BA3" s="233"/>
+      <c r="BB3" s="214"/>
+      <c r="BC3" s="213"/>
+      <c r="BD3" s="213"/>
+      <c r="BE3" s="213"/>
+      <c r="BF3" s="213"/>
     </row>
     <row r="4" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
@@ -22488,7 +22479,7 @@
         <v>34</v>
       </c>
       <c r="D4" s="59">
-        <f>ROUND(AV4-36,2)</f>
+        <f t="shared" ref="D4:D15" si="0">ROUND(AV4-36,2)</f>
         <v>14.36</v>
       </c>
       <c r="E4" s="96">
@@ -22590,11 +22581,11 @@
       <c r="AS4" s="71"/>
       <c r="AT4" s="72"/>
       <c r="AU4" s="63">
-        <f>SUMIF(E4:AS4,"&gt;30")</f>
+        <f t="shared" ref="AU4:AU21" si="1">SUMIF(E4:AS4,"&gt;30")</f>
         <v>705</v>
       </c>
       <c r="AV4" s="64">
-        <f>AU4/(AX4+BC4)</f>
+        <f t="shared" ref="AV4:AV21" si="2">AU4/(AX4+BC4)</f>
         <v>50.357142857142854</v>
       </c>
       <c r="AW4" s="102"/>
@@ -22615,18 +22606,18 @@
       </c>
       <c r="BB4" s="133"/>
       <c r="BC4" s="129">
-        <f>COUNTIF(AA4:AS4, "&gt;30")</f>
+        <f t="shared" ref="BC4:BC21" si="3">COUNTIF(AA4:AS4, "&gt;30")</f>
         <v>5</v>
       </c>
       <c r="BD4" s="149">
         <v>0</v>
       </c>
       <c r="BE4" s="129">
-        <f>SUMIF(AB4:AT4, "&lt;30")+BD4</f>
+        <f t="shared" ref="BE4:BE21" si="4">SUMIF(AB4:AT4, "&lt;30")+BD4</f>
         <v>105</v>
       </c>
       <c r="BF4" s="152">
-        <f>(BE4)/BC4</f>
+        <f t="shared" ref="BF4:BF16" si="5">(BE4)/BC4</f>
         <v>21</v>
       </c>
     </row>
@@ -22641,7 +22632,7 @@
         <v>101</v>
       </c>
       <c r="D5" s="68">
-        <f>ROUND(AV5-36,2)</f>
+        <f t="shared" si="0"/>
         <v>20.83</v>
       </c>
       <c r="E5" s="71"/>
@@ -22711,11 +22702,11 @@
         <v>25</v>
       </c>
       <c r="AU5" s="63">
-        <f>SUMIF(E5:AS5,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>341</v>
       </c>
       <c r="AV5" s="64">
-        <f>AU5/(AX5+BC5)</f>
+        <f t="shared" si="2"/>
         <v>56.833333333333336</v>
       </c>
       <c r="AW5" s="102"/>
@@ -22733,18 +22724,18 @@
       </c>
       <c r="BB5" s="133"/>
       <c r="BC5" s="138">
-        <f>COUNTIF(AA5:AS5, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="BD5" s="150">
         <v>0</v>
       </c>
       <c r="BE5" s="138">
-        <f>SUMIF(AB5:AT5, "&lt;30")+BD5</f>
+        <f t="shared" si="4"/>
         <v>119</v>
       </c>
       <c r="BF5" s="153">
-        <f>(BE5)/BC5</f>
+        <f t="shared" si="5"/>
         <v>19.833333333333332</v>
       </c>
     </row>
@@ -22759,7 +22750,7 @@
         <v>34</v>
       </c>
       <c r="D6" s="68">
-        <f>ROUND(AV6-36,2)</f>
+        <f t="shared" si="0"/>
         <v>12.56</v>
       </c>
       <c r="E6" s="79">
@@ -22869,45 +22860,45 @@
       <c r="AS6" s="71"/>
       <c r="AT6" s="72"/>
       <c r="AU6" s="63">
-        <f>SUMIF(E6:AS6,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>777</v>
       </c>
       <c r="AV6" s="64">
-        <f>AU6/(AX6+BC6)</f>
+        <f t="shared" si="2"/>
         <v>48.5625</v>
       </c>
       <c r="AW6" s="102"/>
       <c r="AX6" s="73">
-        <f>COUNTIF(E6:Y6,"&gt;30")</f>
+        <f t="shared" ref="AX6:AX15" si="6">COUNTIF(E6:Y6,"&gt;30")</f>
         <v>11</v>
       </c>
       <c r="AY6" s="104">
         <v>2</v>
       </c>
       <c r="AZ6" s="105">
-        <f>SUMIF(E6:Z6,"&lt;30")+AY6</f>
+        <f t="shared" ref="AZ6:AZ15" si="7">SUMIF(E6:Z6,"&lt;30")+AY6</f>
         <v>206</v>
       </c>
       <c r="BA6" s="114">
-        <f>(AZ6)/AX6</f>
+        <f t="shared" ref="BA6:BA15" si="8">(AZ6)/AX6</f>
         <v>18.727272727272727</v>
       </c>
       <c r="BB6" s="135" t="s">
         <v>108</v>
       </c>
       <c r="BC6" s="138">
-        <f>COUNTIF(AA6:AS6, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD6" s="150">
         <v>3</v>
       </c>
       <c r="BE6" s="138">
-        <f>SUMIF(AB6:AT6, "&lt;30")+BD6</f>
+        <f t="shared" si="4"/>
         <v>99</v>
       </c>
       <c r="BF6" s="153">
-        <f>(BE6)/BC6</f>
+        <f t="shared" si="5"/>
         <v>19.8</v>
       </c>
     </row>
@@ -22922,7 +22913,7 @@
         <v>34</v>
       </c>
       <c r="D7" s="68">
-        <f>ROUND(AV7-36,2)</f>
+        <f t="shared" si="0"/>
         <v>1.71</v>
       </c>
       <c r="E7" s="69">
@@ -22959,7 +22950,7 @@
       </c>
       <c r="Q7" s="74"/>
       <c r="R7" s="72"/>
-      <c r="S7" s="245">
+      <c r="S7" s="187">
         <v>38</v>
       </c>
       <c r="T7" s="95">
@@ -23009,58 +23000,58 @@
       <c r="AN7" s="70">
         <v>18</v>
       </c>
-      <c r="AO7" s="246">
+      <c r="AO7" s="188">
         <v>34</v>
       </c>
       <c r="AP7" s="70">
         <v>22</v>
       </c>
-      <c r="AQ7" s="247">
+      <c r="AQ7" s="189">
         <v>37</v>
       </c>
       <c r="AR7" s="70">
         <v>19</v>
       </c>
-      <c r="AS7" s="248"/>
+      <c r="AS7" s="190"/>
       <c r="AT7" s="72"/>
       <c r="AU7" s="63">
-        <f>SUMIF(E7:AS7,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>528</v>
       </c>
       <c r="AV7" s="64">
-        <f>AU7/(AX7+BC7)</f>
+        <f t="shared" si="2"/>
         <v>37.714285714285715</v>
       </c>
       <c r="AW7" s="102"/>
       <c r="AX7" s="73">
-        <f>COUNTIF(E7:Y7,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="AY7" s="104">
         <v>5</v>
       </c>
       <c r="AZ7" s="105">
-        <f>SUMIF(E7:Z7,"&lt;30")+AY7</f>
+        <f t="shared" si="7"/>
         <v>127</v>
       </c>
       <c r="BA7" s="114">
-        <f>(AZ7)/AX7</f>
+        <f t="shared" si="8"/>
         <v>18.142857142857142</v>
       </c>
       <c r="BB7" s="133"/>
       <c r="BC7" s="138">
-        <f>COUNTIF(AA7:AS7, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="BD7" s="150">
         <v>8</v>
       </c>
       <c r="BE7" s="138">
-        <f>SUMIF(AB7:AT7, "&lt;30")+BD7</f>
+        <f t="shared" si="4"/>
         <v>138</v>
       </c>
       <c r="BF7" s="153">
-        <f>(BE7)/BC7</f>
+        <f t="shared" si="5"/>
         <v>19.714285714285715</v>
       </c>
     </row>
@@ -23075,7 +23066,7 @@
         <v>34</v>
       </c>
       <c r="D8" s="68">
-        <f>ROUND(AV8-36,2)</f>
+        <f t="shared" si="0"/>
         <v>8.5299999999999994</v>
       </c>
       <c r="E8" s="69">
@@ -23181,43 +23172,43 @@
         <v>24</v>
       </c>
       <c r="AU8" s="63">
-        <f>SUMIF(E8:AS8,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>668</v>
       </c>
       <c r="AV8" s="64">
-        <f>AU8/(AX8+BC8)</f>
+        <f t="shared" si="2"/>
         <v>44.533333333333331</v>
       </c>
       <c r="AW8" s="102"/>
       <c r="AX8" s="73">
-        <f>COUNTIF(E8:Y8,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="AY8" s="104">
         <v>2</v>
       </c>
       <c r="AZ8" s="105">
-        <f>SUMIF(E8:Z8,"&lt;30")+AY8</f>
+        <f t="shared" si="7"/>
         <v>126</v>
       </c>
       <c r="BA8" s="114">
-        <f>(AZ8)/AX8</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="BB8" s="134"/>
       <c r="BC8" s="138">
-        <f>COUNTIF(AA8:AS8, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="BD8" s="150">
         <v>2</v>
       </c>
       <c r="BE8" s="138">
-        <f>SUMIF(AB8:AT8, "&lt;30")+BD8</f>
+        <f t="shared" si="4"/>
         <v>155</v>
       </c>
       <c r="BF8" s="153">
-        <f>(BE8)/BC8</f>
+        <f t="shared" si="5"/>
         <v>19.375</v>
       </c>
     </row>
@@ -23232,7 +23223,7 @@
         <v>34</v>
       </c>
       <c r="D9" s="68">
-        <f>ROUND(AV9-36,2)</f>
+        <f t="shared" si="0"/>
         <v>12.31</v>
       </c>
       <c r="E9" s="69">
@@ -23323,50 +23314,50 @@
       </c>
       <c r="AQ9" s="71"/>
       <c r="AR9" s="72"/>
-      <c r="AS9" s="244">
+      <c r="AS9" s="79">
         <v>46</v>
       </c>
-      <c r="AT9" s="243">
+      <c r="AT9" s="70">
         <v>21</v>
       </c>
       <c r="AU9" s="63">
-        <f>SUMIF(E9:AS9,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>628</v>
       </c>
       <c r="AV9" s="64">
-        <f>AU9/(AX9+BC9)</f>
+        <f t="shared" si="2"/>
         <v>48.307692307692307</v>
       </c>
       <c r="AW9" s="102"/>
       <c r="AX9" s="73">
-        <f>COUNTIF(E9:Y9,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="AY9" s="104">
         <v>2</v>
       </c>
       <c r="AZ9" s="105">
-        <f>SUMIF(E9:Z9,"&lt;30")+AY9</f>
+        <f t="shared" si="7"/>
         <v>127</v>
       </c>
       <c r="BA9" s="114">
-        <f>(AZ9)/AX9</f>
+        <f t="shared" si="8"/>
         <v>18.142857142857142</v>
       </c>
       <c r="BB9" s="134"/>
       <c r="BC9" s="138">
-        <f>COUNTIF(AA9:AS9, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="BD9" s="150">
         <v>1</v>
       </c>
       <c r="BE9" s="138">
-        <f>SUMIF(AB9:AT9, "&lt;30")+BD9</f>
+        <f t="shared" si="4"/>
         <v>113</v>
       </c>
       <c r="BF9" s="153">
-        <f>(BE9)/BC9</f>
+        <f t="shared" si="5"/>
         <v>18.833333333333332</v>
       </c>
     </row>
@@ -23381,7 +23372,7 @@
         <v>101</v>
       </c>
       <c r="D10" s="68">
-        <f>ROUND(AV10-36,2)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="E10" s="71"/>
@@ -23463,43 +23454,43 @@
         <v>19</v>
       </c>
       <c r="AU10" s="63">
-        <f>SUMIF(E10:AS10,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>459</v>
       </c>
       <c r="AV10" s="64">
-        <f>AU10/(AX10+BC10)</f>
+        <f t="shared" si="2"/>
         <v>51</v>
       </c>
       <c r="AW10" s="102"/>
       <c r="AX10" s="73">
-        <f>COUNTIF(E10:Y10,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AY10" s="104">
         <v>0</v>
       </c>
       <c r="AZ10" s="105">
-        <f>SUMIF(E10:Z10,"&lt;30")+AY10</f>
+        <f t="shared" si="7"/>
         <v>88</v>
       </c>
       <c r="BA10" s="114">
-        <f>(AZ10)/AX10</f>
+        <f t="shared" si="8"/>
         <v>17.600000000000001</v>
       </c>
       <c r="BB10" s="134"/>
       <c r="BC10" s="138">
-        <f>COUNTIF(AA10:AS10, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="BD10" s="150">
         <v>0</v>
       </c>
       <c r="BE10" s="138">
-        <f>SUMIF(AB10:AT10, "&lt;30")+BD10</f>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="BF10" s="153">
-        <f>(BE10)/BC10</f>
+        <f t="shared" si="5"/>
         <v>18.5</v>
       </c>
     </row>
@@ -23514,7 +23505,7 @@
         <v>34</v>
       </c>
       <c r="D11" s="68">
-        <f>ROUND(AV11-36,2)</f>
+        <f t="shared" si="0"/>
         <v>10.75</v>
       </c>
       <c r="E11" s="71"/>
@@ -23601,52 +23592,52 @@
       <c r="AP11" s="72"/>
       <c r="AQ11" s="71"/>
       <c r="AR11" s="72"/>
-      <c r="AS11" s="242">
+      <c r="AS11" s="69">
         <v>43</v>
       </c>
-      <c r="AT11" s="243">
+      <c r="AT11" s="70">
         <v>22</v>
       </c>
       <c r="AU11" s="63">
-        <f>SUMIF(E11:AS11,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>561</v>
       </c>
       <c r="AV11" s="64">
-        <f>AU11/(AX11+BC11)</f>
+        <f t="shared" si="2"/>
         <v>46.75</v>
       </c>
       <c r="AW11" s="102"/>
       <c r="AX11" s="73">
-        <f>COUNTIF(E11:Y11,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="AY11" s="104">
         <v>2</v>
       </c>
       <c r="AZ11" s="105">
-        <f>SUMIF(E11:Z11,"&lt;30")+AY11</f>
+        <f t="shared" si="7"/>
         <v>115</v>
       </c>
       <c r="BA11" s="114">
-        <f>(AZ11)/AX11</f>
+        <f t="shared" si="8"/>
         <v>19.166666666666668</v>
       </c>
       <c r="BB11" s="135" t="s">
         <v>106</v>
       </c>
       <c r="BC11" s="138">
-        <f>COUNTIF(AA11:AS11, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="BD11" s="150">
         <v>1</v>
       </c>
       <c r="BE11" s="138">
-        <f>SUMIF(AB11:AT11, "&lt;30")+BD11</f>
+        <f t="shared" si="4"/>
         <v>107</v>
       </c>
       <c r="BF11" s="153">
-        <f>(BE11)/BC11</f>
+        <f t="shared" si="5"/>
         <v>17.833333333333332</v>
       </c>
     </row>
@@ -23661,7 +23652,7 @@
         <v>34</v>
       </c>
       <c r="D12" s="68">
-        <f>ROUND(AV12-36,2)</f>
+        <f t="shared" si="0"/>
         <v>21.5</v>
       </c>
       <c r="E12" s="69">
@@ -23751,43 +23742,43 @@
       <c r="AS12" s="71"/>
       <c r="AT12" s="72"/>
       <c r="AU12" s="63">
-        <f>SUMIF(E12:AS12,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>575</v>
       </c>
       <c r="AV12" s="64">
-        <f>AU12/(AX12+BC12)</f>
+        <f t="shared" si="2"/>
         <v>57.5</v>
       </c>
       <c r="AW12" s="102"/>
       <c r="AX12" s="73">
-        <f>COUNTIF(E12:Y12,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="AY12" s="104">
         <v>1</v>
       </c>
       <c r="AZ12" s="105">
-        <f>SUMIF(E12:Z12,"&lt;30")+AY12</f>
+        <f t="shared" si="7"/>
         <v>102</v>
       </c>
       <c r="BA12" s="114">
-        <f>(AZ12)/AX12</f>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="BB12" s="134"/>
       <c r="BC12" s="138">
-        <f>COUNTIF(AA12:AS12, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="BD12" s="150">
         <v>0</v>
       </c>
       <c r="BE12" s="138">
-        <f>SUMIF(AB12:AT12, "&lt;30")+BD12</f>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
       <c r="BF12" s="153">
-        <f>(BE12)/BC12</f>
+        <f t="shared" si="5"/>
         <v>17.75</v>
       </c>
     </row>
@@ -23802,7 +23793,7 @@
         <v>34</v>
       </c>
       <c r="D13" s="68">
-        <f>ROUND(AV13-36,2)</f>
+        <f t="shared" si="0"/>
         <v>14.72</v>
       </c>
       <c r="E13" s="69">
@@ -23920,45 +23911,45 @@
         <v>17</v>
       </c>
       <c r="AU13" s="63">
-        <f>SUMIF(E13:AS13,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>913</v>
       </c>
       <c r="AV13" s="64">
-        <f>AU13/(AX13+BC13)</f>
+        <f t="shared" si="2"/>
         <v>50.722222222222221</v>
       </c>
       <c r="AW13" s="102"/>
       <c r="AX13" s="73">
-        <f>COUNTIF(E13:Y13,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="AY13" s="104">
         <v>1</v>
       </c>
       <c r="AZ13" s="105">
-        <f>SUMIF(E13:Z13,"&lt;30")+AY13</f>
+        <f t="shared" si="7"/>
         <v>189</v>
       </c>
       <c r="BA13" s="114">
-        <f>(AZ13)/AX13</f>
+        <f t="shared" si="8"/>
         <v>18.899999999999999</v>
       </c>
       <c r="BB13" s="135" t="s">
         <v>107</v>
       </c>
       <c r="BC13" s="138">
-        <f>COUNTIF(AA13:AS13, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="BD13" s="150">
         <v>0</v>
       </c>
       <c r="BE13" s="138">
-        <f>SUMIF(AB13:AT13, "&lt;30")+BD13</f>
+        <f t="shared" si="4"/>
         <v>139</v>
       </c>
       <c r="BF13" s="153">
-        <f>(BE13)/BC13</f>
+        <f t="shared" si="5"/>
         <v>17.375</v>
       </c>
     </row>
@@ -23973,7 +23964,7 @@
         <v>34</v>
       </c>
       <c r="D14" s="68">
-        <f>ROUND(AV14-36,2)</f>
+        <f t="shared" si="0"/>
         <v>16.670000000000002</v>
       </c>
       <c r="E14" s="69">
@@ -24067,43 +24058,43 @@
       <c r="AS14" s="71"/>
       <c r="AT14" s="72"/>
       <c r="AU14" s="63">
-        <f>SUMIF(E14:AS14,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>632</v>
       </c>
       <c r="AV14" s="64">
-        <f>AU14/(AX14+BC14)</f>
+        <f t="shared" si="2"/>
         <v>52.666666666666664</v>
       </c>
       <c r="AW14" s="102"/>
       <c r="AX14" s="73">
-        <f>COUNTIF(E14:Y14,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="AY14" s="104">
         <v>0</v>
       </c>
       <c r="AZ14" s="105">
-        <f>SUMIF(E14:Z14,"&lt;30")+AY14</f>
+        <f t="shared" si="7"/>
         <v>146</v>
       </c>
       <c r="BA14" s="114">
-        <f>(AZ14)/AX14</f>
+        <f t="shared" si="8"/>
         <v>18.25</v>
       </c>
       <c r="BB14" s="134"/>
       <c r="BC14" s="138">
-        <f>COUNTIF(AA14:AS14, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="BD14" s="150">
         <v>1</v>
       </c>
       <c r="BE14" s="138">
-        <f>SUMIF(AB14:AT14, "&lt;30")+BD14</f>
+        <f t="shared" si="4"/>
         <v>66</v>
       </c>
       <c r="BF14" s="153">
-        <f>(BE14)/BC14</f>
+        <f t="shared" si="5"/>
         <v>16.5</v>
       </c>
     </row>
@@ -24118,7 +24109,7 @@
         <v>34</v>
       </c>
       <c r="D15" s="68">
-        <f>ROUND(AV15-36,2)</f>
+        <f t="shared" si="0"/>
         <v>21.75</v>
       </c>
       <c r="E15" s="69">
@@ -24221,50 +24212,50 @@
       </c>
       <c r="AQ15" s="71"/>
       <c r="AR15" s="72"/>
-      <c r="AS15" s="242">
+      <c r="AS15" s="69">
         <v>62</v>
       </c>
-      <c r="AT15" s="243">
+      <c r="AT15" s="70">
         <v>13</v>
       </c>
       <c r="AU15" s="63">
-        <f>SUMIF(E15:AS15,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>924</v>
       </c>
       <c r="AV15" s="64">
-        <f>AU15/(AX15+BC15)</f>
+        <f t="shared" si="2"/>
         <v>57.75</v>
       </c>
       <c r="AW15" s="102"/>
       <c r="AX15" s="73">
-        <f>COUNTIF(E15:Y15,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="AY15" s="104">
         <v>0</v>
       </c>
       <c r="AZ15" s="105">
-        <f>SUMIF(E15:Z15,"&lt;30")+AY15</f>
+        <f t="shared" si="7"/>
         <v>166</v>
       </c>
       <c r="BA15" s="114">
-        <f>(AZ15)/AX15</f>
+        <f t="shared" si="8"/>
         <v>18.444444444444443</v>
       </c>
       <c r="BB15" s="134"/>
       <c r="BC15" s="138">
-        <f>COUNTIF(AA15:AS15, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="BD15" s="150">
         <v>0</v>
       </c>
       <c r="BE15" s="138">
-        <f>SUMIF(AB15:AT15, "&lt;30")+BD15</f>
+        <f t="shared" si="4"/>
         <v>114</v>
       </c>
       <c r="BF15" s="153">
-        <f>(BE15)/BC15</f>
+        <f t="shared" si="5"/>
         <v>16.285714285714285</v>
       </c>
     </row>
@@ -24326,11 +24317,11 @@
       <c r="AS16" s="71"/>
       <c r="AT16" s="72"/>
       <c r="AU16" s="63">
-        <f>SUMIF(E16:AS16,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="AV16" s="64">
-        <f>AU16/(AX16+BC16)</f>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="AW16" s="102"/>
@@ -24340,18 +24331,18 @@
       <c r="BA16" s="114"/>
       <c r="BB16" s="134"/>
       <c r="BC16" s="138">
-        <f>COUNTIF(AA16:AS16, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="BD16" s="150">
         <v>0</v>
       </c>
       <c r="BE16" s="138">
-        <f>SUMIF(AB16:AT16, "&lt;30")+BD16</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BF16" s="153">
-        <f>(BE16)/BC16</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -24454,11 +24445,11 @@
       <c r="AS17" s="71"/>
       <c r="AT17" s="72"/>
       <c r="AU17" s="63">
-        <f>SUMIF(E17:AS17,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>399</v>
       </c>
       <c r="AV17" s="64">
-        <f>AU17/(AX17+BC17)</f>
+        <f t="shared" si="2"/>
         <v>44.333333333333336</v>
       </c>
       <c r="AW17" s="102"/>
@@ -24479,14 +24470,14 @@
       </c>
       <c r="BB17" s="136"/>
       <c r="BC17" s="138">
-        <f>COUNTIF(AA17:AS17, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BD17" s="150">
         <v>0</v>
       </c>
       <c r="BE17" s="138">
-        <f>SUMIF(AB17:AT17, "&lt;30")+BD17</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BF17" s="153">
@@ -24553,11 +24544,11 @@
       <c r="AS18" s="71"/>
       <c r="AT18" s="72"/>
       <c r="AU18" s="63">
-        <f>SUMIF(E18:AS18,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="AV18" s="64">
-        <f>AU18/(AX18+BC18)</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="AW18" s="102"/>
@@ -24578,14 +24569,14 @@
       </c>
       <c r="BB18" s="134"/>
       <c r="BC18" s="138">
-        <f>COUNTIF(AA18:AS18, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BD18" s="150">
         <v>0</v>
       </c>
       <c r="BE18" s="138">
-        <f>SUMIF(AB18:AT18, "&lt;30")+BD18</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BF18" s="153">
@@ -24652,11 +24643,11 @@
       <c r="AS19" s="71"/>
       <c r="AT19" s="72"/>
       <c r="AU19" s="63">
-        <f>SUMIF(E19:AS19,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="AV19" s="64">
-        <f>AU19/(AX19+BC19)</f>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="AW19" s="102"/>
@@ -24677,14 +24668,14 @@
       </c>
       <c r="BB19" s="134"/>
       <c r="BC19" s="138">
-        <f>COUNTIF(AA19:AS19, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BD19" s="138">
         <v>0</v>
       </c>
       <c r="BE19" s="138">
-        <f>SUMIF(AB19:AT19, "&lt;30")+BD19</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BF19" s="153">
@@ -24764,11 +24755,11 @@
       <c r="AS20" s="71"/>
       <c r="AT20" s="72"/>
       <c r="AU20" s="63">
-        <f>SUMIF(E20:AS20,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>217</v>
       </c>
       <c r="AV20" s="64">
-        <f>AU20/(AX20+BC20)</f>
+        <f t="shared" si="2"/>
         <v>54.25</v>
       </c>
       <c r="AW20" s="102"/>
@@ -24789,14 +24780,14 @@
       </c>
       <c r="BB20" s="134"/>
       <c r="BC20" s="138">
-        <f>COUNTIF(AA20:AS20, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BD20" s="150">
         <v>0</v>
       </c>
       <c r="BE20" s="138">
-        <f>SUMIF(AB20:AT20, "&lt;30")+BD20</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BF20" s="153">
@@ -24867,11 +24858,11 @@
       <c r="AS21" s="71"/>
       <c r="AT21" s="72"/>
       <c r="AU21" s="63">
-        <f>SUMIF(E21:AS21,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>123</v>
       </c>
       <c r="AV21" s="64">
-        <f>AU21/(AX21+BC21)</f>
+        <f t="shared" si="2"/>
         <v>61.5</v>
       </c>
       <c r="AW21" s="102"/>
@@ -24892,14 +24883,14 @@
       </c>
       <c r="BB21" s="137"/>
       <c r="BC21" s="139">
-        <f>COUNTIF(AA21:AS21, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="BD21" s="151">
         <v>0</v>
       </c>
       <c r="BE21" s="139">
-        <f>SUMIF(AB21:AT21, "&lt;30")+BD21</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BF21" s="154">
@@ -25126,6 +25117,48 @@
     <sortCondition ref="AV4:AV21"/>
   </sortState>
   <mergeCells count="58">
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AU1:AU3"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AS1:AT1"/>
+    <mergeCell ref="AS2:AT2"/>
     <mergeCell ref="BB1:BB3"/>
     <mergeCell ref="AM1:AN1"/>
     <mergeCell ref="AM2:AN2"/>
@@ -25142,48 +25175,6 @@
     <mergeCell ref="BA2:BA3"/>
     <mergeCell ref="AQ1:AR1"/>
     <mergeCell ref="AQ2:AR2"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="AU1:AU3"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="AO2:AP2"/>
-    <mergeCell ref="AS1:AT1"/>
-    <mergeCell ref="AS2:AT2"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="AI1:AJ1"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="AA2:AB2"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26342,23 +26333,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -26372,23 +26363,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -27914,23 +27905,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -27944,23 +27935,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -29575,23 +29566,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -29605,23 +29596,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -31027,23 +31018,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -31057,23 +31048,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -32422,23 +32413,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -32452,23 +32443,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -33225,9 +33216,9 @@
       </c>
       <c r="O15" s="17"/>
       <c r="P15" s="38"/>
-      <c r="Q15" s="238"/>
-      <c r="R15" s="239"/>
-      <c r="S15" s="240"/>
+      <c r="Q15" s="250"/>
+      <c r="R15" s="251"/>
+      <c r="S15" s="252"/>
       <c r="T15" s="43">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
09/24/24 commit - update to overall
</commit_message>
<xml_diff>
--- a/public/results/Bottoms Up 2024 League Stats - Week 21.xlsx
+++ b/public/results/Bottoms Up 2024 League Stats - Week 21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\CODE\golf-league-site\public\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECE393D-A9A6-47A7-911B-D8686E5E4F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29799116-83C9-49D0-BC1A-2B39D622AA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="720" windowWidth="20400" windowHeight="13695" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4410" yWindow="915" windowWidth="20400" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OVERALL" sheetId="30" r:id="rId1"/>
@@ -1520,7 +1520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="254">
+  <cellXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1991,9 +1991,6 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2055,6 +2052,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -2682,8 +2685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCFEFA5-64DE-44E8-8682-4097340CFE3F}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2697,39 +2700,39 @@
     <col min="7" max="7" width="3.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="8.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="185" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="184" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="199"/>
-      <c r="B1" s="200"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="202"/>
-      <c r="H1" s="203" t="s">
+      <c r="A1" s="200"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="202"/>
+      <c r="E1" s="202"/>
+      <c r="F1" s="203"/>
+      <c r="H1" s="204" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="204"/>
-      <c r="J1" s="205"/>
+      <c r="I1" s="205"/>
+      <c r="J1" s="206"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="163"/>
       <c r="B2" s="164"/>
-      <c r="C2" s="206" t="s">
+      <c r="C2" s="207" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="207"/>
-      <c r="E2" s="206" t="s">
+      <c r="D2" s="208"/>
+      <c r="E2" s="207" t="s">
         <v>125</v>
       </c>
-      <c r="F2" s="207"/>
-      <c r="H2" s="206" t="s">
+      <c r="F2" s="208"/>
+      <c r="H2" s="207" t="s">
         <v>126</v>
       </c>
-      <c r="I2" s="208"/>
-      <c r="J2" s="207"/>
+      <c r="I2" s="209"/>
+      <c r="J2" s="208"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="165"/>
@@ -2766,10 +2769,10 @@
       <c r="C4" s="173">
         <v>0</v>
       </c>
-      <c r="D4" s="191">
+      <c r="D4" s="190">
         <v>0</v>
       </c>
-      <c r="E4" s="186">
+      <c r="E4" s="185">
         <v>119</v>
       </c>
       <c r="F4" s="174">
@@ -2779,11 +2782,11 @@
         <f t="shared" ref="H4:H21" si="0">C4+E4</f>
         <v>119</v>
       </c>
-      <c r="I4" s="194">
+      <c r="I4" s="193">
         <f t="shared" ref="I4:I21" si="1">D4+F4</f>
         <v>6</v>
       </c>
-      <c r="J4" s="176">
+      <c r="J4" s="197">
         <f t="shared" ref="J4:J21" si="2">H4/I4</f>
         <v>19.833333333333332</v>
       </c>
@@ -2795,19 +2798,19 @@
       <c r="B5" s="164" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="177">
+      <c r="C5" s="176">
         <v>166</v>
       </c>
-      <c r="D5" s="178">
+      <c r="D5" s="177">
         <v>9</v>
       </c>
-      <c r="E5" s="179">
+      <c r="E5" s="178">
         <v>105</v>
       </c>
-      <c r="F5" s="192">
-        <v>5</v>
-      </c>
-      <c r="H5" s="180">
+      <c r="F5" s="191">
+        <v>5</v>
+      </c>
+      <c r="H5" s="179">
         <f t="shared" si="0"/>
         <v>271</v>
       </c>
@@ -2815,7 +2818,7 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="J5" s="181">
+      <c r="J5" s="198">
         <f t="shared" si="2"/>
         <v>19.357142857142858</v>
       </c>
@@ -2827,19 +2830,19 @@
       <c r="B6" s="164" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="177">
+      <c r="C6" s="176">
         <v>206</v>
       </c>
-      <c r="D6" s="178">
+      <c r="D6" s="177">
         <v>11</v>
       </c>
-      <c r="E6" s="177">
+      <c r="E6" s="176">
         <v>99</v>
       </c>
-      <c r="F6" s="192">
-        <v>5</v>
-      </c>
-      <c r="H6" s="180">
+      <c r="F6" s="191">
+        <v>5</v>
+      </c>
+      <c r="H6" s="179">
         <f t="shared" si="0"/>
         <v>305</v>
       </c>
@@ -2847,7 +2850,7 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="J6" s="181">
+      <c r="J6" s="198">
         <f t="shared" si="2"/>
         <v>19.0625</v>
       </c>
@@ -2859,19 +2862,19 @@
       <c r="B7" s="164" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="177">
+      <c r="C7" s="176">
         <v>127</v>
       </c>
-      <c r="D7" s="178">
+      <c r="D7" s="177">
         <v>7</v>
       </c>
-      <c r="E7" s="179">
+      <c r="E7" s="178">
         <v>138</v>
       </c>
-      <c r="F7" s="178">
+      <c r="F7" s="177">
         <v>7</v>
       </c>
-      <c r="H7" s="180">
+      <c r="H7" s="179">
         <f t="shared" si="0"/>
         <v>265</v>
       </c>
@@ -2879,7 +2882,7 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="J7" s="181">
+      <c r="J7" s="198">
         <f t="shared" si="2"/>
         <v>18.928571428571427</v>
       </c>
@@ -2891,27 +2894,27 @@
       <c r="B8" s="164" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="177">
+      <c r="C8" s="176">
         <v>169</v>
       </c>
-      <c r="D8" s="178">
+      <c r="D8" s="177">
         <v>9</v>
       </c>
-      <c r="E8" s="179">
+      <c r="E8" s="178">
         <v>0</v>
       </c>
-      <c r="F8" s="192">
+      <c r="F8" s="191">
         <v>0</v>
       </c>
-      <c r="H8" s="180">
+      <c r="H8" s="179">
         <f t="shared" si="0"/>
         <v>169</v>
       </c>
-      <c r="I8" s="195">
+      <c r="I8" s="194">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="J8" s="181">
+      <c r="J8" s="198">
         <f t="shared" si="2"/>
         <v>18.777777777777779</v>
       </c>
@@ -2923,19 +2926,19 @@
       <c r="B9" s="164" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="177">
+      <c r="C9" s="176">
         <v>126</v>
       </c>
-      <c r="D9" s="178">
+      <c r="D9" s="177">
         <v>7</v>
       </c>
-      <c r="E9" s="179">
+      <c r="E9" s="178">
         <v>155</v>
       </c>
-      <c r="F9" s="178">
+      <c r="F9" s="177">
         <v>8</v>
       </c>
-      <c r="H9" s="180">
+      <c r="H9" s="179">
         <f t="shared" si="0"/>
         <v>281</v>
       </c>
@@ -2943,7 +2946,7 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="J9" s="181">
+      <c r="J9" s="198">
         <f t="shared" si="2"/>
         <v>18.733333333333334</v>
       </c>
@@ -2955,19 +2958,19 @@
       <c r="B10" s="164" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="177">
+      <c r="C10" s="176">
         <v>115</v>
       </c>
-      <c r="D10" s="178">
-        <v>6</v>
-      </c>
-      <c r="E10" s="179">
+      <c r="D10" s="177">
+        <v>6</v>
+      </c>
+      <c r="E10" s="178">
         <v>107</v>
       </c>
-      <c r="F10" s="178">
-        <v>6</v>
-      </c>
-      <c r="H10" s="180">
+      <c r="F10" s="177">
+        <v>6</v>
+      </c>
+      <c r="H10" s="179">
         <f t="shared" si="0"/>
         <v>222</v>
       </c>
@@ -2975,7 +2978,7 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="J10" s="181">
+      <c r="J10" s="198">
         <f t="shared" si="2"/>
         <v>18.5</v>
       </c>
@@ -2987,19 +2990,19 @@
       <c r="B11" s="164" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="177">
+      <c r="C11" s="176">
         <v>127</v>
       </c>
-      <c r="D11" s="178">
+      <c r="D11" s="177">
         <v>7</v>
       </c>
-      <c r="E11" s="179">
+      <c r="E11" s="178">
         <v>113</v>
       </c>
-      <c r="F11" s="178">
-        <v>6</v>
-      </c>
-      <c r="H11" s="180">
+      <c r="F11" s="177">
+        <v>6</v>
+      </c>
+      <c r="H11" s="179">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
@@ -3007,7 +3010,7 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="J11" s="181">
+      <c r="J11" s="198">
         <f t="shared" si="2"/>
         <v>18.46153846153846</v>
       </c>
@@ -3019,19 +3022,19 @@
       <c r="B12" s="164" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="177">
+      <c r="C12" s="176">
         <v>189</v>
       </c>
-      <c r="D12" s="178">
+      <c r="D12" s="177">
         <v>10</v>
       </c>
-      <c r="E12" s="179">
+      <c r="E12" s="178">
         <v>139</v>
       </c>
-      <c r="F12" s="178">
+      <c r="F12" s="177">
         <v>8</v>
       </c>
-      <c r="H12" s="180">
+      <c r="H12" s="179">
         <f t="shared" si="0"/>
         <v>328</v>
       </c>
@@ -3039,7 +3042,7 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="J12" s="181">
+      <c r="J12" s="198">
         <f t="shared" si="2"/>
         <v>18.222222222222221</v>
       </c>
@@ -3051,27 +3054,27 @@
       <c r="B13" s="164" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="177">
+      <c r="C13" s="176">
         <v>88</v>
       </c>
-      <c r="D13" s="192">
-        <v>5</v>
-      </c>
-      <c r="E13" s="179">
+      <c r="D13" s="191">
+        <v>5</v>
+      </c>
+      <c r="E13" s="178">
         <v>74</v>
       </c>
-      <c r="F13" s="192">
-        <v>4</v>
-      </c>
-      <c r="H13" s="180">
+      <c r="F13" s="191">
+        <v>4</v>
+      </c>
+      <c r="H13" s="179">
         <f t="shared" si="0"/>
         <v>162</v>
       </c>
-      <c r="I13" s="195">
+      <c r="I13" s="194">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="J13" s="181">
+      <c r="J13" s="198">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
@@ -3083,27 +3086,27 @@
       <c r="B14" s="164" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="177">
+      <c r="C14" s="176">
         <v>72</v>
       </c>
-      <c r="D14" s="192">
-        <v>4</v>
-      </c>
-      <c r="E14" s="179">
+      <c r="D14" s="191">
+        <v>4</v>
+      </c>
+      <c r="E14" s="178">
         <v>0</v>
       </c>
-      <c r="F14" s="192">
+      <c r="F14" s="191">
         <v>0</v>
       </c>
-      <c r="H14" s="180">
+      <c r="H14" s="179">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="I14" s="195">
+      <c r="I14" s="194">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="J14" s="181">
+      <c r="J14" s="198">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
@@ -3115,19 +3118,19 @@
       <c r="B15" s="164" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="177">
+      <c r="C15" s="176">
         <v>146</v>
       </c>
-      <c r="D15" s="178">
+      <c r="D15" s="177">
         <v>8</v>
       </c>
-      <c r="E15" s="179">
+      <c r="E15" s="178">
         <v>66</v>
       </c>
-      <c r="F15" s="192">
-        <v>4</v>
-      </c>
-      <c r="H15" s="180">
+      <c r="F15" s="191">
+        <v>4</v>
+      </c>
+      <c r="H15" s="179">
         <f t="shared" si="0"/>
         <v>212</v>
       </c>
@@ -3135,7 +3138,7 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="J15" s="181">
+      <c r="J15" s="198">
         <f t="shared" si="2"/>
         <v>17.666666666666668</v>
       </c>
@@ -3147,19 +3150,19 @@
       <c r="B16" s="164" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="177">
+      <c r="C16" s="176">
         <v>166</v>
       </c>
-      <c r="D16" s="178">
+      <c r="D16" s="177">
         <v>9</v>
       </c>
-      <c r="E16" s="179">
+      <c r="E16" s="178">
         <v>114</v>
       </c>
-      <c r="F16" s="178">
+      <c r="F16" s="177">
         <v>7</v>
       </c>
-      <c r="H16" s="180">
+      <c r="H16" s="179">
         <f t="shared" si="0"/>
         <v>280</v>
       </c>
@@ -3167,7 +3170,7 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="J16" s="181">
+      <c r="J16" s="198">
         <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
@@ -3179,27 +3182,27 @@
       <c r="B17" s="164" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="177">
+      <c r="C17" s="176">
         <v>102</v>
       </c>
-      <c r="D17" s="178">
-        <v>6</v>
-      </c>
-      <c r="E17" s="179">
+      <c r="D17" s="177">
+        <v>6</v>
+      </c>
+      <c r="E17" s="178">
         <v>71</v>
       </c>
-      <c r="F17" s="192">
-        <v>4</v>
-      </c>
-      <c r="H17" s="180">
+      <c r="F17" s="191">
+        <v>4</v>
+      </c>
+      <c r="H17" s="179">
         <f t="shared" si="0"/>
         <v>173</v>
       </c>
-      <c r="I17" s="195">
+      <c r="I17" s="194">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="J17" s="181">
+      <c r="J17" s="198">
         <f t="shared" si="2"/>
         <v>17.3</v>
       </c>
@@ -3211,27 +3214,27 @@
       <c r="B18" s="164" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="177">
+      <c r="C18" s="176">
         <v>0</v>
       </c>
-      <c r="D18" s="192">
-        <v>1</v>
-      </c>
-      <c r="E18" s="179">
+      <c r="D18" s="191">
+        <v>1</v>
+      </c>
+      <c r="E18" s="178">
         <v>0</v>
       </c>
-      <c r="F18" s="192">
-        <v>1</v>
-      </c>
-      <c r="H18" s="180">
+      <c r="F18" s="191">
+        <v>1</v>
+      </c>
+      <c r="H18" s="179">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I18" s="195">
+      <c r="I18" s="194">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="J18" s="181">
+      <c r="J18" s="180">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3243,27 +3246,27 @@
       <c r="B19" s="164" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="177">
+      <c r="C19" s="176">
         <v>0</v>
       </c>
-      <c r="D19" s="192">
-        <v>1</v>
-      </c>
-      <c r="E19" s="179">
+      <c r="D19" s="191">
+        <v>1</v>
+      </c>
+      <c r="E19" s="178">
         <v>0</v>
       </c>
-      <c r="F19" s="192">
+      <c r="F19" s="191">
         <v>0</v>
       </c>
-      <c r="H19" s="180">
+      <c r="H19" s="179">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I19" s="195">
+      <c r="I19" s="194">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J19" s="181">
+      <c r="J19" s="180">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3275,27 +3278,27 @@
       <c r="B20" s="164" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="177">
+      <c r="C20" s="176">
         <v>0</v>
       </c>
-      <c r="D20" s="192">
+      <c r="D20" s="191">
         <v>0</v>
       </c>
-      <c r="E20" s="179">
+      <c r="E20" s="178">
         <v>0</v>
       </c>
-      <c r="F20" s="192">
-        <v>1</v>
-      </c>
-      <c r="H20" s="180">
+      <c r="F20" s="191">
+        <v>1</v>
+      </c>
+      <c r="H20" s="179">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I20" s="195">
+      <c r="I20" s="194">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J20" s="181">
+      <c r="J20" s="180">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3307,23 +3310,23 @@
       <c r="B21" s="166" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="182">
+      <c r="C21" s="181">
         <v>0</v>
       </c>
-      <c r="D21" s="193">
-        <v>1</v>
-      </c>
-      <c r="E21" s="183">
+      <c r="D21" s="192">
+        <v>1</v>
+      </c>
+      <c r="E21" s="182">
         <v>0</v>
       </c>
-      <c r="F21" s="193">
+      <c r="F21" s="192">
         <v>0</v>
       </c>
-      <c r="H21" s="184">
+      <c r="H21" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I21" s="196">
+      <c r="I21" s="195">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3333,12 +3336,12 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="197"/>
-      <c r="D23" s="198" t="s">
+      <c r="C23" s="196"/>
+      <c r="D23" s="199" t="s">
         <v>131</v>
       </c>
-      <c r="E23" s="198"/>
-      <c r="F23" s="198"/>
+      <c r="E23" s="199"/>
+      <c r="F23" s="199"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J21">
@@ -3387,23 +3390,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -3417,23 +3420,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -5061,23 +5064,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -5091,23 +5094,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -6116,23 +6119,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -6146,23 +6149,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -7168,23 +7171,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -7198,23 +7201,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -8605,23 +8608,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -8635,23 +8638,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -9657,23 +9660,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -9687,23 +9690,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -10606,23 +10609,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -10636,23 +10639,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -11972,23 +11975,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -12002,23 +12005,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -13329,24 +13332,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="253" t="s">
+      <c r="A1" s="254" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="253"/>
-      <c r="C1" s="253"/>
-      <c r="D1" s="253"/>
+      <c r="B1" s="254"/>
+      <c r="C1" s="254"/>
+      <c r="D1" s="254"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="253"/>
-      <c r="B2" s="253"/>
-      <c r="C2" s="253"/>
-      <c r="D2" s="253"/>
+      <c r="A2" s="254"/>
+      <c r="B2" s="254"/>
+      <c r="C2" s="254"/>
+      <c r="D2" s="254"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="253"/>
-      <c r="B3" s="253"/>
-      <c r="C3" s="253"/>
-      <c r="D3" s="253"/>
+      <c r="A3" s="254"/>
+      <c r="B3" s="254"/>
+      <c r="C3" s="254"/>
+      <c r="D3" s="254"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -13383,23 +13386,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -13413,23 +13416,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -14755,23 +14758,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -14785,23 +14788,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -15644,24 +15647,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="253" t="s">
+      <c r="A1" s="254" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="253"/>
-      <c r="C1" s="253"/>
-      <c r="D1" s="253"/>
+      <c r="B1" s="254"/>
+      <c r="C1" s="254"/>
+      <c r="D1" s="254"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="253"/>
-      <c r="B2" s="253"/>
-      <c r="C2" s="253"/>
-      <c r="D2" s="253"/>
+      <c r="A2" s="254"/>
+      <c r="B2" s="254"/>
+      <c r="C2" s="254"/>
+      <c r="D2" s="254"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="253"/>
-      <c r="B3" s="253"/>
-      <c r="C3" s="253"/>
-      <c r="D3" s="253"/>
+      <c r="A3" s="254"/>
+      <c r="B3" s="254"/>
+      <c r="C3" s="254"/>
+      <c r="D3" s="254"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -15698,23 +15701,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -15728,23 +15731,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -17068,23 +17071,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -17098,23 +17101,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -18391,23 +18394,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -18421,23 +18424,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -19714,23 +19717,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -19744,23 +19747,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -21003,7 +21006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC67D2C9-51E9-4325-BE9D-6FFAA314D9FD}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
@@ -21026,23 +21029,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -21056,23 +21059,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -22091,244 +22094,244 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" s="1" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="237" t="s">
+      <c r="A1" s="238" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="243"/>
-      <c r="D1" s="246" t="s">
+      <c r="B1" s="239"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="247" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="215" t="s">
+      <c r="E1" s="216" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="216"/>
-      <c r="G1" s="215" t="s">
+      <c r="F1" s="217"/>
+      <c r="G1" s="216" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="216"/>
-      <c r="I1" s="215" t="s">
+      <c r="H1" s="217"/>
+      <c r="I1" s="216" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="216"/>
-      <c r="K1" s="215" t="s">
+      <c r="J1" s="217"/>
+      <c r="K1" s="216" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="216"/>
-      <c r="M1" s="215" t="s">
+      <c r="L1" s="217"/>
+      <c r="M1" s="216" t="s">
         <v>70</v>
       </c>
-      <c r="N1" s="216"/>
-      <c r="O1" s="215" t="s">
+      <c r="N1" s="217"/>
+      <c r="O1" s="216" t="s">
         <v>84</v>
       </c>
-      <c r="P1" s="216"/>
-      <c r="Q1" s="215" t="s">
+      <c r="P1" s="217"/>
+      <c r="Q1" s="216" t="s">
         <v>89</v>
       </c>
-      <c r="R1" s="216"/>
-      <c r="S1" s="215" t="s">
+      <c r="R1" s="217"/>
+      <c r="S1" s="216" t="s">
         <v>90</v>
       </c>
-      <c r="T1" s="216"/>
-      <c r="U1" s="215" t="s">
+      <c r="T1" s="217"/>
+      <c r="U1" s="216" t="s">
         <v>93</v>
       </c>
-      <c r="V1" s="216"/>
-      <c r="W1" s="215" t="s">
+      <c r="V1" s="217"/>
+      <c r="W1" s="216" t="s">
         <v>95</v>
       </c>
-      <c r="X1" s="216"/>
-      <c r="Y1" s="215" t="s">
+      <c r="X1" s="217"/>
+      <c r="Y1" s="216" t="s">
         <v>96</v>
       </c>
-      <c r="Z1" s="216"/>
-      <c r="AA1" s="215" t="s">
+      <c r="Z1" s="217"/>
+      <c r="AA1" s="216" t="s">
         <v>105</v>
       </c>
-      <c r="AB1" s="216"/>
-      <c r="AC1" s="215" t="s">
+      <c r="AB1" s="217"/>
+      <c r="AC1" s="216" t="s">
         <v>110</v>
       </c>
-      <c r="AD1" s="216"/>
-      <c r="AE1" s="215" t="s">
+      <c r="AD1" s="217"/>
+      <c r="AE1" s="216" t="s">
         <v>112</v>
       </c>
-      <c r="AF1" s="216"/>
-      <c r="AG1" s="215" t="s">
+      <c r="AF1" s="217"/>
+      <c r="AG1" s="216" t="s">
         <v>113</v>
       </c>
-      <c r="AH1" s="216"/>
-      <c r="AI1" s="215" t="s">
+      <c r="AH1" s="217"/>
+      <c r="AI1" s="216" t="s">
         <v>115</v>
       </c>
-      <c r="AJ1" s="216"/>
-      <c r="AK1" s="215" t="s">
+      <c r="AJ1" s="217"/>
+      <c r="AK1" s="216" t="s">
         <v>116</v>
       </c>
-      <c r="AL1" s="216"/>
-      <c r="AM1" s="215" t="s">
+      <c r="AL1" s="217"/>
+      <c r="AM1" s="216" t="s">
         <v>118</v>
       </c>
-      <c r="AN1" s="216"/>
-      <c r="AO1" s="215" t="s">
+      <c r="AN1" s="217"/>
+      <c r="AO1" s="216" t="s">
         <v>119</v>
       </c>
-      <c r="AP1" s="216"/>
-      <c r="AQ1" s="215" t="s">
+      <c r="AP1" s="217"/>
+      <c r="AQ1" s="216" t="s">
         <v>120</v>
       </c>
-      <c r="AR1" s="216"/>
-      <c r="AS1" s="215" t="s">
+      <c r="AR1" s="217"/>
+      <c r="AS1" s="216" t="s">
         <v>129</v>
       </c>
-      <c r="AT1" s="216"/>
-      <c r="AU1" s="234" t="s">
+      <c r="AT1" s="217"/>
+      <c r="AU1" s="235" t="s">
         <v>35</v>
       </c>
-      <c r="AV1" s="222" t="s">
+      <c r="AV1" s="223" t="s">
         <v>111</v>
       </c>
       <c r="AW1" s="112"/>
-      <c r="AX1" s="225" t="s">
+      <c r="AX1" s="226" t="s">
         <v>103</v>
       </c>
-      <c r="AY1" s="226"/>
-      <c r="AZ1" s="226"/>
-      <c r="BA1" s="227"/>
-      <c r="BB1" s="212" t="s">
+      <c r="AY1" s="227"/>
+      <c r="AZ1" s="227"/>
+      <c r="BA1" s="228"/>
+      <c r="BB1" s="213" t="s">
         <v>109</v>
       </c>
-      <c r="BC1" s="219" t="s">
+      <c r="BC1" s="220" t="s">
         <v>104</v>
       </c>
-      <c r="BD1" s="220"/>
-      <c r="BE1" s="220"/>
-      <c r="BF1" s="221"/>
+      <c r="BD1" s="221"/>
+      <c r="BE1" s="221"/>
+      <c r="BF1" s="222"/>
     </row>
     <row r="2" spans="1:58" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="239"/>
-      <c r="B2" s="240"/>
-      <c r="C2" s="244"/>
-      <c r="D2" s="247"/>
-      <c r="E2" s="217">
+      <c r="A2" s="240"/>
+      <c r="B2" s="241"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="248"/>
+      <c r="E2" s="218">
         <v>45418</v>
       </c>
-      <c r="F2" s="218"/>
-      <c r="G2" s="248">
+      <c r="F2" s="219"/>
+      <c r="G2" s="249">
         <v>45425</v>
       </c>
-      <c r="H2" s="249"/>
-      <c r="I2" s="248">
+      <c r="H2" s="250"/>
+      <c r="I2" s="249">
         <v>45432</v>
       </c>
-      <c r="J2" s="249"/>
-      <c r="K2" s="248">
+      <c r="J2" s="250"/>
+      <c r="K2" s="249">
         <v>45439</v>
       </c>
-      <c r="L2" s="249"/>
-      <c r="M2" s="248">
+      <c r="L2" s="250"/>
+      <c r="M2" s="249">
         <v>45446</v>
       </c>
-      <c r="N2" s="249"/>
-      <c r="O2" s="248">
+      <c r="N2" s="250"/>
+      <c r="O2" s="249">
         <v>45453</v>
       </c>
-      <c r="P2" s="249"/>
-      <c r="Q2" s="248">
+      <c r="P2" s="250"/>
+      <c r="Q2" s="249">
         <v>45460</v>
       </c>
-      <c r="R2" s="249"/>
-      <c r="S2" s="248">
+      <c r="R2" s="250"/>
+      <c r="S2" s="249">
         <v>45467</v>
       </c>
-      <c r="T2" s="249"/>
-      <c r="U2" s="248">
+      <c r="T2" s="250"/>
+      <c r="U2" s="249">
         <v>45474</v>
       </c>
-      <c r="V2" s="249"/>
-      <c r="W2" s="248">
+      <c r="V2" s="250"/>
+      <c r="W2" s="249">
         <v>45481</v>
       </c>
-      <c r="X2" s="249"/>
-      <c r="Y2" s="248">
+      <c r="X2" s="250"/>
+      <c r="Y2" s="249">
         <v>45488</v>
       </c>
-      <c r="Z2" s="249"/>
-      <c r="AA2" s="217">
+      <c r="Z2" s="250"/>
+      <c r="AA2" s="218">
         <v>45495</v>
       </c>
-      <c r="AB2" s="218"/>
-      <c r="AC2" s="217">
+      <c r="AB2" s="219"/>
+      <c r="AC2" s="218">
         <v>45502</v>
       </c>
-      <c r="AD2" s="218"/>
-      <c r="AE2" s="217">
+      <c r="AD2" s="219"/>
+      <c r="AE2" s="218">
         <v>45509</v>
       </c>
-      <c r="AF2" s="218"/>
-      <c r="AG2" s="217">
+      <c r="AF2" s="219"/>
+      <c r="AG2" s="218">
         <v>45516</v>
       </c>
-      <c r="AH2" s="218"/>
-      <c r="AI2" s="217">
+      <c r="AH2" s="219"/>
+      <c r="AI2" s="218">
         <v>45523</v>
       </c>
-      <c r="AJ2" s="218"/>
-      <c r="AK2" s="217">
+      <c r="AJ2" s="219"/>
+      <c r="AK2" s="218">
         <v>45530</v>
       </c>
-      <c r="AL2" s="218"/>
-      <c r="AM2" s="217">
+      <c r="AL2" s="219"/>
+      <c r="AM2" s="218">
         <v>45537</v>
       </c>
-      <c r="AN2" s="218"/>
-      <c r="AO2" s="217">
+      <c r="AN2" s="219"/>
+      <c r="AO2" s="218">
         <v>45544</v>
       </c>
-      <c r="AP2" s="218"/>
-      <c r="AQ2" s="217">
+      <c r="AP2" s="219"/>
+      <c r="AQ2" s="218">
         <v>45551</v>
       </c>
-      <c r="AR2" s="218"/>
-      <c r="AS2" s="217">
+      <c r="AR2" s="219"/>
+      <c r="AS2" s="218">
         <v>45558</v>
       </c>
-      <c r="AT2" s="218"/>
-      <c r="AU2" s="235"/>
-      <c r="AV2" s="223"/>
+      <c r="AT2" s="219"/>
+      <c r="AU2" s="236"/>
+      <c r="AV2" s="224"/>
       <c r="AW2" s="112"/>
-      <c r="AX2" s="228" t="s">
+      <c r="AX2" s="229" t="s">
         <v>88</v>
       </c>
-      <c r="AY2" s="230" t="s">
+      <c r="AY2" s="231" t="s">
         <v>102</v>
       </c>
-      <c r="AZ2" s="230" t="s">
+      <c r="AZ2" s="231" t="s">
         <v>36</v>
       </c>
-      <c r="BA2" s="232" t="s">
+      <c r="BA2" s="233" t="s">
         <v>61</v>
       </c>
-      <c r="BB2" s="213"/>
-      <c r="BC2" s="212" t="s">
+      <c r="BB2" s="214"/>
+      <c r="BC2" s="213" t="s">
         <v>88</v>
       </c>
-      <c r="BD2" s="212" t="s">
+      <c r="BD2" s="213" t="s">
         <v>102</v>
       </c>
-      <c r="BE2" s="212" t="s">
+      <c r="BE2" s="213" t="s">
         <v>36</v>
       </c>
-      <c r="BF2" s="212" t="s">
+      <c r="BF2" s="213" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:58" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="241"/>
-      <c r="B3" s="242"/>
-      <c r="C3" s="245"/>
-      <c r="D3" s="247"/>
+      <c r="A3" s="242"/>
+      <c r="B3" s="243"/>
+      <c r="C3" s="246"/>
+      <c r="D3" s="248"/>
       <c r="E3" s="52" t="s">
         <v>26</v>
       </c>
@@ -22455,18 +22458,18 @@
       <c r="AT3" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="AU3" s="236"/>
-      <c r="AV3" s="224"/>
+      <c r="AU3" s="237"/>
+      <c r="AV3" s="225"/>
       <c r="AW3" s="112"/>
-      <c r="AX3" s="229"/>
-      <c r="AY3" s="231"/>
-      <c r="AZ3" s="231"/>
-      <c r="BA3" s="233"/>
-      <c r="BB3" s="214"/>
-      <c r="BC3" s="213"/>
-      <c r="BD3" s="213"/>
-      <c r="BE3" s="213"/>
-      <c r="BF3" s="213"/>
+      <c r="AX3" s="230"/>
+      <c r="AY3" s="232"/>
+      <c r="AZ3" s="232"/>
+      <c r="BA3" s="234"/>
+      <c r="BB3" s="215"/>
+      <c r="BC3" s="214"/>
+      <c r="BD3" s="214"/>
+      <c r="BE3" s="214"/>
+      <c r="BF3" s="214"/>
     </row>
     <row r="4" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
@@ -22950,7 +22953,7 @@
       </c>
       <c r="Q7" s="74"/>
       <c r="R7" s="72"/>
-      <c r="S7" s="187">
+      <c r="S7" s="186">
         <v>38</v>
       </c>
       <c r="T7" s="95">
@@ -23000,19 +23003,19 @@
       <c r="AN7" s="70">
         <v>18</v>
       </c>
-      <c r="AO7" s="188">
+      <c r="AO7" s="187">
         <v>34</v>
       </c>
       <c r="AP7" s="70">
         <v>22</v>
       </c>
-      <c r="AQ7" s="189">
+      <c r="AQ7" s="188">
         <v>37</v>
       </c>
       <c r="AR7" s="70">
         <v>19</v>
       </c>
-      <c r="AS7" s="190"/>
+      <c r="AS7" s="189"/>
       <c r="AT7" s="72"/>
       <c r="AU7" s="63">
         <f t="shared" si="1"/>
@@ -26333,23 +26336,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -26363,23 +26366,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -27905,23 +27908,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -27935,23 +27938,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -29566,23 +29569,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -29596,23 +29599,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -31018,23 +31021,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -31048,23 +31051,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -32413,23 +32416,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -32443,23 +32446,23 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="211"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -33216,9 +33219,9 @@
       </c>
       <c r="O15" s="17"/>
       <c r="P15" s="38"/>
-      <c r="Q15" s="250"/>
-      <c r="R15" s="251"/>
-      <c r="S15" s="252"/>
+      <c r="Q15" s="251"/>
+      <c r="R15" s="252"/>
+      <c r="S15" s="253"/>
       <c r="T15" s="43">
         <v>35</v>
       </c>

</xml_diff>